<commit_message>
Added link to online asset list
</commit_message>
<xml_diff>
--- a/Asset list.xlsx
+++ b/Asset list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bryan.levee\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bryan.levee\Desktop\New folder\Team-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,6 +21,20 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Arttt</t>
+  </si>
+  <si>
+    <t>Sound</t>
+  </si>
+  <si>
+    <t>Game</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -336,14 +350,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>